<commit_message>
error fixes -fixed uncorrected age calculation -fixed isotope masses -added function for printing list (for debugging)
</commit_message>
<xml_diff>
--- a/data/CPR_100221_20210210-114741/Results.xlsx
+++ b/data/CPR_100221_20210210-114741/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="135">
   <si>
     <t>Lab. #</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Ch. Bl. 230</t>
   </si>
   <si>
-    <t>Sp. Bl. 230</t>
-  </si>
-  <si>
     <t>230Th1</t>
   </si>
   <si>
@@ -354,9 +351,6 @@
     <t>(ng/g)</t>
   </si>
   <si>
-    <t>(fg/g)</t>
-  </si>
-  <si>
     <t>(dpmg/g)</t>
   </si>
   <si>
@@ -372,13 +366,13 @@
     <t>(ka)</t>
   </si>
   <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Akt. Ver. initial</t>
+  </si>
+  <si>
     <t>Out of range</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>Akt. Ver. initial</t>
   </si>
   <si>
     <t>Taylor 1. Ord.</t>
@@ -1887,7 +1881,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BG13"/>
+  <dimension ref="A1:BF13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1910,7 +1904,7 @@
     <col min="15" max="15" width="19.7109375" customWidth="1"/>
     <col min="16" max="16" width="23.7109375" customWidth="1"/>
     <col min="17" max="17" width="19.7109375" customWidth="1"/>
-    <col min="18" max="18" width="21.7109375" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" customWidth="1"/>
     <col min="19" max="19" width="19.7109375" customWidth="1"/>
     <col min="20" max="20" width="23.7109375" customWidth="1"/>
     <col min="21" max="21" width="19.7109375" customWidth="1"/>
@@ -1921,40 +1915,39 @@
     <col min="26" max="26" width="23.7109375" customWidth="1"/>
     <col min="27" max="27" width="23.7109375" customWidth="1"/>
     <col min="28" max="28" width="12.7109375" customWidth="1"/>
-    <col min="29" max="29" width="12.7109375" customWidth="1"/>
-    <col min="30" max="30" width="21.7109375" customWidth="1"/>
+    <col min="29" max="29" width="21.7109375" customWidth="1"/>
+    <col min="30" max="30" width="22.7109375" customWidth="1"/>
     <col min="31" max="31" width="22.7109375" customWidth="1"/>
     <col min="32" max="32" width="22.7109375" customWidth="1"/>
-    <col min="33" max="33" width="22.7109375" customWidth="1"/>
+    <col min="33" max="33" width="19.7109375" customWidth="1"/>
     <col min="34" max="34" width="19.7109375" customWidth="1"/>
-    <col min="35" max="35" width="19.7109375" customWidth="1"/>
+    <col min="35" max="35" width="20.7109375" customWidth="1"/>
     <col min="36" max="36" width="20.7109375" customWidth="1"/>
-    <col min="37" max="37" width="20.7109375" customWidth="1"/>
-    <col min="38" max="38" width="22.7109375" customWidth="1"/>
-    <col min="39" max="39" width="23.7109375" customWidth="1"/>
-    <col min="40" max="40" width="22.7109375" customWidth="1"/>
-    <col min="41" max="41" width="23.7109375" customWidth="1"/>
-    <col min="42" max="42" width="16.7109375" customWidth="1"/>
-    <col min="43" max="43" width="9.7109375" customWidth="1"/>
-    <col min="44" max="44" width="19.7109375" customWidth="1"/>
+    <col min="37" max="37" width="22.7109375" customWidth="1"/>
+    <col min="38" max="38" width="23.7109375" customWidth="1"/>
+    <col min="39" max="39" width="22.7109375" customWidth="1"/>
+    <col min="40" max="40" width="23.7109375" customWidth="1"/>
+    <col min="41" max="41" width="16.7109375" customWidth="1"/>
+    <col min="42" max="42" width="9.7109375" customWidth="1"/>
+    <col min="43" max="43" width="19.7109375" customWidth="1"/>
+    <col min="44" max="44" width="23.7109375" customWidth="1"/>
     <col min="45" max="45" width="23.7109375" customWidth="1"/>
-    <col min="46" max="46" width="23.7109375" customWidth="1"/>
-    <col min="47" max="47" width="18.7109375" customWidth="1"/>
-    <col min="48" max="48" width="9.7109375" customWidth="1"/>
-    <col min="49" max="49" width="13.7109375" customWidth="1"/>
-    <col min="50" max="50" width="13.7109375" customWidth="1"/>
-    <col min="51" max="51" width="22.7109375" customWidth="1"/>
-    <col min="52" max="52" width="19.7109375" customWidth="1"/>
-    <col min="53" max="53" width="12.7109375" customWidth="1"/>
-    <col min="54" max="54" width="6.7109375" customWidth="1"/>
-    <col min="55" max="55" width="19.7109375" customWidth="1"/>
-    <col min="56" max="56" width="20.7109375" customWidth="1"/>
+    <col min="46" max="46" width="18.7109375" customWidth="1"/>
+    <col min="47" max="47" width="9.7109375" customWidth="1"/>
+    <col min="48" max="48" width="13.7109375" customWidth="1"/>
+    <col min="49" max="49" width="14.7109375" customWidth="1"/>
+    <col min="50" max="50" width="22.7109375" customWidth="1"/>
+    <col min="51" max="51" width="19.7109375" customWidth="1"/>
+    <col min="52" max="52" width="12.7109375" customWidth="1"/>
+    <col min="53" max="53" width="6.7109375" customWidth="1"/>
+    <col min="54" max="54" width="19.7109375" customWidth="1"/>
+    <col min="55" max="55" width="20.7109375" customWidth="1"/>
+    <col min="56" max="56" width="18.7109375" customWidth="1"/>
     <col min="57" max="57" width="19.7109375" customWidth="1"/>
     <col min="58" max="58" width="19.7109375" customWidth="1"/>
-    <col min="59" max="59" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="1" customFormat="1">
+    <row r="1" spans="1:58" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1965,61 +1958,61 @@
         <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>58</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>63</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>67</v>
@@ -2028,100 +2021,100 @@
         <v>68</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>125</v>
+        <v>83</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>88</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="BA1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="BB1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="BC1" s="1" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>100</v>
@@ -2129,178 +2122,172 @@
       <c r="BF1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="BG1" s="1" t="s">
-        <v>102</v>
-      </c>
     </row>
-    <row r="2" spans="1:59" s="3" customFormat="1">
+    <row r="2" spans="1:58" s="3" customFormat="1">
       <c r="C2" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="BC2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="AG2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="BF2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AS2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="BB2" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="BC2" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="BE2" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="BF2" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="BG2" s="3" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="3" spans="1:59" s="4" customFormat="1">
+    <row r="3" spans="1:58" s="4" customFormat="1">
       <c r="A3" s="4">
         <v>10815</v>
       </c>
@@ -2350,10 +2337,10 @@
         <v>0.001458381816529189</v>
       </c>
       <c r="Q3" s="4">
-        <v>10.40023165849734</v>
+        <v>10.2229084183414</v>
       </c>
       <c r="R3" s="4">
-        <v>0.06620424170825219</v>
+        <v>0.001088158080050232</v>
       </c>
       <c r="S3" s="4">
         <v>1.000114366734304</v>
@@ -2371,112 +2358,109 @@
         <v>0</v>
       </c>
       <c r="X3" s="4">
-        <v>0.9308953049971663</v>
+        <v>0.9284286765323656</v>
       </c>
       <c r="Y3" s="4">
-        <v>0.004344705994292121</v>
+        <v>0.004333193662648399</v>
       </c>
       <c r="Z3" s="4">
-        <v>0.0002273033307682513</v>
+        <v>0.0002267010365437481</v>
       </c>
       <c r="AA3" s="4">
-        <v>1.06087777906925E-06</v>
+        <v>1.058066731131335E-06</v>
       </c>
       <c r="AB3" s="4">
         <v>0</v>
       </c>
       <c r="AC3" s="4">
-        <v>0.85</v>
+        <v>224.1086737872328</v>
       </c>
       <c r="AD3" s="4">
-        <v>224.6961553523945</v>
+        <v>0.7639864796420964</v>
       </c>
       <c r="AE3" s="4">
-        <v>0.7659892043257855</v>
+        <v>10.2170232939209</v>
       </c>
       <c r="AF3" s="4">
-        <v>10.24380633955038</v>
+        <v>0.0348298328968497</v>
       </c>
       <c r="AG3" s="4">
-        <v>0.03492113630067952</v>
+        <v>45068.26898406901</v>
       </c>
       <c r="AH3" s="4">
-        <v>45066.6794231648</v>
+        <v>260.4788137042241</v>
       </c>
       <c r="AI3" s="4">
-        <v>260.4696265987955</v>
+        <v>0.1143667343042054</v>
       </c>
       <c r="AJ3" s="4">
-        <v>0.1143667343042054</v>
+        <v>1.672089322806292</v>
       </c>
       <c r="AK3" s="4">
-        <v>1.672089322806292</v>
+        <v>0.9994243199508722</v>
       </c>
       <c r="AL3" s="4">
-        <v>1.002044224632932</v>
+        <v>0.003408697990423883</v>
       </c>
       <c r="AM3" s="4">
-        <v>0.003417633598299904</v>
+        <v>0.9994243199508722</v>
       </c>
       <c r="AN3" s="4">
-        <v>1.002044224632932</v>
+        <v>0.003408697990423883</v>
       </c>
       <c r="AO3" s="4">
-        <v>0.003417633598299903</v>
+        <v>787.196</v>
       </c>
       <c r="AP3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR3" s="4">
+        <v>2.217578670048665E-05</v>
+      </c>
+      <c r="AS3" s="4">
+        <v>1.035264937069868E-07</v>
+      </c>
+      <c r="AT3" s="4">
+        <v>8</v>
+      </c>
+      <c r="AU3" s="4">
+        <v>4</v>
+      </c>
+      <c r="AV3" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="AQ3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AR3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AS3" s="4">
-        <v>2.223470283275118E-05</v>
-      </c>
-      <c r="AT3" s="4">
-        <v>1.038015405713216E-07</v>
-      </c>
-      <c r="AU3" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="AV3" s="4">
-        <v>0.375</v>
-      </c>
       <c r="AW3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AX3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AY3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AZ3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BB3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BC3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BD3" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="AX3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AY3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AZ3" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BA3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BC3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="BD3" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="BE3" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="BF3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="BG3" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:58">
       <c r="A4">
         <v>10989</v>
       </c>
@@ -2526,10 +2510,10 @@
         <v>0.0001619437037934368</v>
       </c>
       <c r="Q4">
-        <v>2.494533049558064</v>
+        <v>2.151004382936691</v>
       </c>
       <c r="R4">
-        <v>0.006844932384407318</v>
+        <v>0.0001208327941275882</v>
       </c>
       <c r="S4">
         <v>1.146015048919254</v>
@@ -2547,115 +2531,112 @@
         <v>0.003</v>
       </c>
       <c r="X4">
-        <v>0.1648649603714585</v>
+        <v>0.164348706667991</v>
       </c>
       <c r="Y4">
-        <v>0.0003275915424590783</v>
+        <v>0.0003265657311123974</v>
       </c>
       <c r="Z4">
-        <v>4.025625053455646E-05</v>
+        <v>4.013019319417705E-05</v>
       </c>
       <c r="AA4">
-        <v>7.999035802708682E-08</v>
+        <v>7.973987837100867E-08</v>
       </c>
       <c r="AB4">
         <v>0.05</v>
       </c>
       <c r="AC4">
-        <v>0.85</v>
+        <v>0.06097318120314129</v>
       </c>
       <c r="AD4">
-        <v>0.06025788678615855</v>
+        <v>0.001291801527102739</v>
       </c>
       <c r="AE4">
-        <v>0.001276647021433962</v>
+        <v>0.002779742533519217</v>
       </c>
       <c r="AF4">
-        <v>0.002747132551956153</v>
+        <v>5.889270625045821E-05</v>
       </c>
       <c r="AG4">
-        <v>5.820181850029131E-05</v>
+        <v>69.26810743394481</v>
       </c>
       <c r="AH4">
-        <v>68.24114306418033</v>
+        <v>1.473981315707428</v>
       </c>
       <c r="AI4">
-        <v>1.452128166415402</v>
+        <v>145.9064109889343</v>
       </c>
       <c r="AJ4">
-        <v>145.9064109889343</v>
+        <v>0.5483315951927344</v>
       </c>
       <c r="AK4">
-        <v>0.5483315951927344</v>
+        <v>0.001292299799837754</v>
       </c>
       <c r="AL4">
-        <v>0.001277139448784195</v>
+        <v>2.737926232677275E-05</v>
       </c>
       <c r="AM4">
-        <v>2.705806810503453E-05</v>
+        <v>0.001293671958225894</v>
       </c>
       <c r="AN4">
-        <v>0.001275152828087398</v>
+        <v>2.740833351015257E-05</v>
       </c>
       <c r="AO4">
-        <v>2.701597863848178E-05</v>
+        <v>0.1232</v>
       </c>
       <c r="AP4">
-        <v>0.1218</v>
+        <v>0.0041</v>
       </c>
       <c r="AQ4">
-        <v>0.0032</v>
+        <v>3.327922077922078</v>
       </c>
       <c r="AR4">
-        <v>2.627257799671593</v>
+        <v>1.865649066664787E-05</v>
       </c>
       <c r="AS4">
-        <v>1.871509461063766E-05</v>
+        <v>3.708580901895586E-08</v>
       </c>
       <c r="AT4">
-        <v>3.720230331112454E-08</v>
+        <v>8</v>
       </c>
       <c r="AU4">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV4">
-        <v>0.375</v>
+        <v>0.1091</v>
       </c>
       <c r="AW4">
-        <v>0.1202</v>
+        <v>0.0076270048</v>
       </c>
       <c r="AX4">
-        <v>0.0026814172</v>
+        <v>0.007577624118811419</v>
       </c>
       <c r="AY4">
-        <v>0.002663187902121503</v>
-      </c>
-      <c r="AZ4">
-        <v>2.230796339434276</v>
-      </c>
-      <c r="BA4" t="s">
+        <v>6.990838496791933</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>26</v>
       </c>
+      <c r="BA4">
+        <v>30</v>
+      </c>
       <c r="BB4">
-        <v>30</v>
+        <v>145.9514080700588</v>
       </c>
       <c r="BC4">
-        <v>145.9559869192395</v>
+        <v>0.5485097219309453</v>
       </c>
       <c r="BD4">
-        <v>0.5485190220285382</v>
+        <v>51.10000000000001</v>
       </c>
       <c r="BE4">
-        <v>62.2</v>
+        <v>3.788812059405709</v>
       </c>
       <c r="BF4">
-        <v>1.331593951060752</v>
-      </c>
-      <c r="BG4">
-        <v>1107.815267105451</v>
+        <v>6.945576644190118</v>
       </c>
     </row>
-    <row r="5" spans="1:59" s="4" customFormat="1">
+    <row r="5" spans="1:58" s="4" customFormat="1">
       <c r="A5" s="4">
         <v>10815</v>
       </c>
@@ -2705,10 +2686,10 @@
         <v>0.001718799455033931</v>
       </c>
       <c r="Q5" s="4">
-        <v>10.34489129641446</v>
+        <v>10.22317599622057</v>
       </c>
       <c r="R5" s="4">
-        <v>0.08830543895282254</v>
+        <v>0.001282466288171574</v>
       </c>
       <c r="S5" s="4">
         <v>1.00007524374222</v>
@@ -2726,112 +2707,109 @@
         <v>0</v>
       </c>
       <c r="X5" s="4">
-        <v>0.9350241754877243</v>
+        <v>0.9325466065987698</v>
       </c>
       <c r="Y5" s="4">
-        <v>0.003866776386707385</v>
+        <v>0.003856530443204103</v>
       </c>
       <c r="Z5" s="4">
-        <v>0.0002283115064565124</v>
+        <v>0.0002277065408307927</v>
       </c>
       <c r="AA5" s="4">
-        <v>9.441783058915393E-07</v>
+        <v>9.416764809573525E-07</v>
       </c>
       <c r="AB5" s="4">
         <v>0</v>
       </c>
       <c r="AC5" s="4">
-        <v>0.85</v>
+        <v>223.8970280920027</v>
       </c>
       <c r="AD5" s="4">
-        <v>224.4839473616327</v>
+        <v>0.6387388207707742</v>
       </c>
       <c r="AE5" s="4">
-        <v>0.640413198163658</v>
+        <v>10.20737445275075</v>
       </c>
       <c r="AF5" s="4">
-        <v>10.23413186355563</v>
+        <v>0.02911984306659327</v>
       </c>
       <c r="AG5" s="4">
-        <v>0.02919617725097272</v>
+        <v>44826.88294990959</v>
       </c>
       <c r="AH5" s="4">
-        <v>44825.30040817269</v>
+        <v>225.2113611056301</v>
       </c>
       <c r="AI5" s="4">
-        <v>225.203410377069</v>
+        <v>0.07524374222045438</v>
       </c>
       <c r="AJ5" s="4">
-        <v>0.07524374222045438</v>
+        <v>1.847658475256469</v>
       </c>
       <c r="AK5" s="4">
-        <v>1.847658475256469</v>
+        <v>0.9984543410506036</v>
       </c>
       <c r="AL5" s="4">
-        <v>1.001071669639563</v>
+        <v>0.002851167071869993</v>
       </c>
       <c r="AM5" s="4">
-        <v>0.002858641065203783</v>
+        <v>0.9984543410506036</v>
       </c>
       <c r="AN5" s="4">
-        <v>1.001071669639563</v>
+        <v>0.002851167071869993</v>
       </c>
       <c r="AO5" s="4">
-        <v>0.002858641065203783</v>
+        <v>699.4166</v>
       </c>
       <c r="AP5" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AQ5" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AR5" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="AR5" s="4">
+        <v>2.227356165197333E-05</v>
       </c>
       <c r="AS5" s="4">
-        <v>2.233273755053395E-05</v>
+        <v>9.215430044876766E-08</v>
       </c>
       <c r="AT5" s="4">
-        <v>9.239913392535709E-08</v>
+        <v>8</v>
       </c>
       <c r="AU5" s="4">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV5" s="4">
-        <v>0.375</v>
+        <v>699.3971</v>
       </c>
       <c r="AW5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="AX5" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="AX5" s="4">
+        <v>256.5464924142581</v>
       </c>
       <c r="AY5" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AZ5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BA5" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="BB5" s="4">
+        <v>0.5431789176196203</v>
+      </c>
       <c r="BC5" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="BD5" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="BE5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BF5" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="BG5" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="BD5" s="4">
+        <v>699339.1</v>
+      </c>
+      <c r="BE5" s="4">
+        <v>128273.2462071291</v>
+      </c>
+      <c r="BF5" s="4">
+        <v>36.68109181668871</v>
       </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:58">
       <c r="A6">
         <v>10990</v>
       </c>
@@ -2881,10 +2859,10 @@
         <v>0.0001723385360822908</v>
       </c>
       <c r="Q6">
-        <v>2.498781508865185</v>
+        <v>2.159505325145284</v>
       </c>
       <c r="R6">
-        <v>0.007131896276153311</v>
+        <v>0.0001285888019286201</v>
       </c>
       <c r="S6">
         <v>1.145956643442365</v>
@@ -2902,115 +2880,112 @@
         <v>0.003</v>
       </c>
       <c r="X6">
-        <v>0.08206535589386277</v>
+        <v>0.08175910603621016</v>
       </c>
       <c r="Y6">
-        <v>0.0002542747168099036</v>
+        <v>0.0002533258194953242</v>
       </c>
       <c r="Z6">
-        <v>2.003848191651771E-05</v>
+        <v>1.996370270953486E-05</v>
       </c>
       <c r="AA6">
-        <v>6.208806699397941E-08</v>
+        <v>6.185636798443117E-08</v>
       </c>
       <c r="AB6">
         <v>0.05</v>
       </c>
       <c r="AC6">
-        <v>0.85</v>
+        <v>0.05779578540821469</v>
       </c>
       <c r="AD6">
-        <v>0.05697928276837074</v>
+        <v>0.001154479715308004</v>
       </c>
       <c r="AE6">
-        <v>0.001138169949318366</v>
+        <v>0.002634886351461793</v>
       </c>
       <c r="AF6">
-        <v>0.002597662328179437</v>
+        <v>5.263226069892974E-05</v>
       </c>
       <c r="AG6">
-        <v>5.188870510057422E-05</v>
+        <v>131.9838503807886</v>
       </c>
       <c r="AH6">
-        <v>129.6336887695163</v>
+        <v>2.667925870214171</v>
       </c>
       <c r="AI6">
-        <v>2.620419626504751</v>
+        <v>144.4746150985909</v>
       </c>
       <c r="AJ6">
-        <v>144.4746150985909</v>
+        <v>0.4966198109484972</v>
       </c>
       <c r="AK6">
-        <v>0.4966198109484972</v>
+        <v>0.001220134222769062</v>
       </c>
       <c r="AL6">
-        <v>0.001202896931038906</v>
+        <v>2.437247731538343E-05</v>
       </c>
       <c r="AM6">
-        <v>2.402815822832558E-05</v>
+        <v>0.001222639286764136</v>
       </c>
       <c r="AN6">
-        <v>0.001202215160090243</v>
+        <v>2.442251657684677E-05</v>
       </c>
       <c r="AO6">
-        <v>2.40145396881105E-05</v>
+        <v>0.1163</v>
       </c>
       <c r="AP6">
-        <v>0.1147</v>
+        <v>0.0044</v>
       </c>
       <c r="AQ6">
-        <v>0.0052</v>
+        <v>3.783319002579536</v>
       </c>
       <c r="AR6">
-        <v>4.533565823888405</v>
+        <v>9.244572114306674E-06</v>
       </c>
       <c r="AS6">
-        <v>9.279200047895037E-06</v>
+        <v>2.864905625561545E-08</v>
       </c>
       <c r="AT6">
-        <v>2.875636869854111E-08</v>
+        <v>8</v>
       </c>
       <c r="AU6">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV6">
-        <v>0.375</v>
+        <v>0.1097</v>
       </c>
       <c r="AW6">
-        <v>0.1141</v>
+        <v>0.0042628134</v>
       </c>
       <c r="AX6">
-        <v>0.0023327735</v>
+        <v>0.0042299295372283</v>
       </c>
       <c r="AY6">
-        <v>0.002318047539323532</v>
-      </c>
-      <c r="AZ6">
-        <v>2.044499123575811</v>
-      </c>
-      <c r="BA6" t="s">
+        <v>3.885882771194166</v>
+      </c>
+      <c r="AZ6" t="s">
         <v>27</v>
       </c>
+      <c r="BA6">
+        <v>47.5</v>
+      </c>
       <c r="BB6">
-        <v>47.5</v>
+        <v>144.5194156912648</v>
       </c>
       <c r="BC6">
-        <v>144.5212129054278</v>
+        <v>0.4967768607109589</v>
       </c>
       <c r="BD6">
-        <v>0.4967809009411691</v>
+        <v>51.7</v>
       </c>
       <c r="BE6">
-        <v>56.09999999999999</v>
+        <v>2.11496476861415</v>
       </c>
       <c r="BF6">
-        <v>1.159023769661766</v>
-      </c>
-      <c r="BG6">
-        <v>1015.796467714081</v>
+        <v>3.855906597291066</v>
       </c>
     </row>
-    <row r="7" spans="1:59" s="4" customFormat="1">
+    <row r="7" spans="1:58" s="4" customFormat="1">
       <c r="A7" s="4">
         <v>10815</v>
       </c>
@@ -3060,10 +3035,10 @@
         <v>0.001771577620583448</v>
       </c>
       <c r="Q7" s="4">
-        <v>10.51311112792597</v>
+        <v>10.22472872482657</v>
       </c>
       <c r="R7" s="4">
-        <v>0.07231692961550673</v>
+        <v>0.00132184622739052</v>
       </c>
       <c r="S7" s="4">
         <v>1.002514640426851</v>
@@ -3081,112 +3056,109 @@
         <v>0</v>
       </c>
       <c r="X7" s="4">
-        <v>0.9446978553457307</v>
+        <v>0.9421946537417234</v>
       </c>
       <c r="Y7" s="4">
-        <v>0.00359360536525734</v>
+        <v>0.003584083253331734</v>
       </c>
       <c r="Z7" s="4">
-        <v>0.0002306735977042681</v>
+        <v>0.0002300623731561144</v>
       </c>
       <c r="AA7" s="4">
-        <v>8.77476193729582E-07</v>
+        <v>8.751511119024211E-07</v>
       </c>
       <c r="AB7" s="4">
         <v>0</v>
       </c>
       <c r="AC7" s="4">
-        <v>0.85</v>
+        <v>223.7053034071008</v>
       </c>
       <c r="AD7" s="4">
-        <v>224.2917133068922</v>
+        <v>0.4943297527625418</v>
       </c>
       <c r="AE7" s="4">
-        <v>0.4956255640659236</v>
+        <v>10.19863380233968</v>
       </c>
       <c r="AF7" s="4">
-        <v>10.22536799118078</v>
+        <v>0.02253629238664822</v>
       </c>
       <c r="AG7" s="4">
-        <v>0.02259536789696849</v>
+        <v>44329.86438603393</v>
       </c>
       <c r="AH7" s="4">
-        <v>44328.29804948058</v>
+        <v>195.0168804580674</v>
       </c>
       <c r="AI7" s="4">
-        <v>195.0099897970511</v>
+        <v>2.514640426850789</v>
       </c>
       <c r="AJ7" s="4">
-        <v>2.514640426850789</v>
+        <v>1.802158364614082</v>
       </c>
       <c r="AK7" s="4">
-        <v>1.802158364614082</v>
+        <v>0.9974478616314266</v>
       </c>
       <c r="AL7" s="4">
-        <v>1.000062521595576</v>
+        <v>0.002207865684017097</v>
       </c>
       <c r="AM7" s="4">
-        <v>0.002213653272754594</v>
+        <v>0.9974478616314266</v>
       </c>
       <c r="AN7" s="4">
-        <v>1.000062521595576</v>
+        <v>0.002207865684017097</v>
       </c>
       <c r="AO7" s="4">
-        <v>0.002213653272754594</v>
-      </c>
-      <c r="AP7" s="4">
-        <v>617.4591</v>
+        <v>557.1646</v>
+      </c>
+      <c r="AP7" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="AQ7" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AR7" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="AR7" s="4">
+        <v>2.250058454827287E-05</v>
       </c>
       <c r="AS7" s="4">
-        <v>2.256036359616776E-05</v>
+        <v>8.564103664792728E-08</v>
       </c>
       <c r="AT7" s="4">
-        <v>8.586856583147189E-08</v>
+        <v>8</v>
       </c>
       <c r="AU7" s="4">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV7" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="AW7" s="4">
-        <v>617.4573</v>
-      </c>
-      <c r="AX7" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AY7" s="4">
-        <v>103.9089916358842</v>
+        <v>557.1452</v>
+      </c>
+      <c r="AW7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AX7" s="4">
+        <v>59.5616806850411</v>
+      </c>
+      <c r="AY7" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="AZ7" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BA7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="BC7" s="4">
-        <v>14.40030502845515</v>
-      </c>
-      <c r="BD7" s="4" t="s">
-        <v>119</v>
+      <c r="BB7" s="4">
+        <v>12.14344236039566</v>
+      </c>
+      <c r="BC7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BD7" s="4">
+        <v>557087.2000000001</v>
       </c>
       <c r="BE7" s="4">
-        <v>617399.3</v>
+        <v>29780.84034252055</v>
       </c>
       <c r="BF7" s="4">
-        <v>51954.49581794211</v>
-      </c>
-      <c r="BG7" s="4">
-        <v>8414.265378017573</v>
+        <v>10.69051311669581</v>
       </c>
     </row>
-    <row r="8" spans="1:59">
+    <row r="8" spans="1:58">
       <c r="A8">
         <v>10991</v>
       </c>
@@ -3236,10 +3208,10 @@
         <v>0.0001972308851365691</v>
       </c>
       <c r="Q8">
-        <v>2.391626369770513</v>
+        <v>2.056093993624354</v>
       </c>
       <c r="R8">
-        <v>0.008333495916921346</v>
+        <v>0.000147161997540252</v>
       </c>
       <c r="S8">
         <v>1.146358704091157</v>
@@ -3257,115 +3229,112 @@
         <v>0.003</v>
       </c>
       <c r="X8">
-        <v>0.06829703125084907</v>
+        <v>0.06804359221735705</v>
       </c>
       <c r="Y8">
-        <v>0.0002631033824980844</v>
+        <v>0.0002621270491824548</v>
       </c>
       <c r="Z8">
-        <v>1.667657211457157E-05</v>
+        <v>1.661468810231995E-05</v>
       </c>
       <c r="AA8">
-        <v>6.424382511886218E-08</v>
+        <v>6.400542686570602E-08</v>
       </c>
       <c r="AB8">
         <v>0.05</v>
       </c>
       <c r="AC8">
-        <v>0.85</v>
+        <v>0.06191767674622532</v>
       </c>
       <c r="AD8">
-        <v>0.06128399097454247</v>
+        <v>0.001198934509509678</v>
       </c>
       <c r="AE8">
-        <v>0.001186664221285368</v>
+        <v>0.00282280170120612</v>
       </c>
       <c r="AF8">
-        <v>0.002793912224592392</v>
+        <v>5.465893668700942E-05</v>
       </c>
       <c r="AG8">
-        <v>5.409953923713687E-05</v>
+        <v>169.8979652113942</v>
       </c>
       <c r="AH8">
-        <v>167.5351628258868</v>
+        <v>3.354271162584406</v>
       </c>
       <c r="AI8">
-        <v>3.307622693930106</v>
+        <v>144.5202595351331</v>
       </c>
       <c r="AJ8">
-        <v>144.5202595351331</v>
+        <v>0.5464885728009569</v>
       </c>
       <c r="AK8">
-        <v>0.5464885728009569</v>
+        <v>0.001372895261578126</v>
       </c>
       <c r="AL8">
-        <v>0.001358844602073594</v>
+        <v>2.658405221541558E-05</v>
       </c>
       <c r="AM8">
-        <v>2.631198232313543E-05</v>
+        <v>0.00137769211062768</v>
       </c>
       <c r="AN8">
-        <v>0.001360027298009095</v>
+        <v>2.667693598388037E-05</v>
       </c>
       <c r="AO8">
-        <v>2.633488345141829E-05</v>
+        <v>0.1309</v>
       </c>
       <c r="AP8">
-        <v>0.1295</v>
+        <v>0.0026</v>
       </c>
       <c r="AQ8">
-        <v>0.0026</v>
+        <v>1.986249045072574</v>
       </c>
       <c r="AR8">
-        <v>2.007722007722008</v>
+        <v>8.080704556231217E-06</v>
       </c>
       <c r="AS8">
-        <v>8.110802408004294E-06</v>
+        <v>3.113499337914811E-08</v>
       </c>
       <c r="AT8">
-        <v>3.125096054626335E-08</v>
+        <v>8</v>
       </c>
       <c r="AU8">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV8">
-        <v>0.375</v>
+        <v>0.1254</v>
       </c>
       <c r="AW8">
-        <v>0.1293</v>
+        <v>0.0040577034</v>
       </c>
       <c r="AX8">
-        <v>0.0025250226</v>
+        <v>0.004000928025806783</v>
       </c>
       <c r="AY8">
-        <v>0.002532899142229332</v>
-      </c>
-      <c r="AZ8">
-        <v>1.952840371229698</v>
-      </c>
-      <c r="BA8" t="s">
+        <v>3.235808133971292</v>
+      </c>
+      <c r="AZ8" t="s">
         <v>28</v>
       </c>
+      <c r="BA8">
+        <v>70</v>
+      </c>
       <c r="BB8">
-        <v>70</v>
+        <v>144.5714891971889</v>
       </c>
       <c r="BC8">
-        <v>144.5730827553311</v>
+        <v>0.5466848067060551</v>
       </c>
       <c r="BD8">
-        <v>0.5466892919830495</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="BE8">
-        <v>71.30000000000001</v>
+        <v>2.000464012903391</v>
       </c>
       <c r="BF8">
-        <v>1.266449571114666</v>
-      </c>
-      <c r="BG8">
-        <v>979.4660256107239</v>
+        <v>3.190532715954372</v>
       </c>
     </row>
-    <row r="9" spans="1:59" s="4" customFormat="1">
+    <row r="9" spans="1:58" s="4" customFormat="1">
       <c r="A9" s="4">
         <v>10815</v>
       </c>
@@ -3415,10 +3384,10 @@
         <v>0.001644691398066958</v>
       </c>
       <c r="Q9" s="4">
-        <v>10.43349082855542</v>
+        <v>10.22386654656593</v>
       </c>
       <c r="R9" s="4">
-        <v>0.0889522643630432</v>
+        <v>0.001227171248099452</v>
       </c>
       <c r="S9" s="4">
         <v>1.000697962479403</v>
@@ -3436,112 +3405,109 @@
         <v>0</v>
       </c>
       <c r="X9" s="4">
-        <v>0.9488419428341529</v>
+        <v>0.9463277604849375</v>
       </c>
       <c r="Y9" s="4">
-        <v>0.004077997428984894</v>
+        <v>0.004067191805104615</v>
       </c>
       <c r="Z9" s="4">
-        <v>0.0002316854890351801</v>
+        <v>0.0002310715832403312</v>
       </c>
       <c r="AA9" s="4">
-        <v>9.957536508098015E-07</v>
+        <v>9.9311516473534E-07</v>
       </c>
       <c r="AB9" s="4">
         <v>0</v>
       </c>
       <c r="AC9" s="4">
-        <v>0.85</v>
+        <v>223.2694701586305</v>
       </c>
       <c r="AD9" s="4">
-        <v>223.8547221464317</v>
+        <v>0.5191415766427769</v>
       </c>
       <c r="AE9" s="4">
-        <v>0.5205023925190567</v>
+        <v>10.17876434179344</v>
       </c>
       <c r="AF9" s="4">
-        <v>10.20544574189782</v>
+        <v>0.0236674533464855</v>
       </c>
       <c r="AG9" s="4">
-        <v>0.0237294923888471</v>
+        <v>44050.2644204709</v>
       </c>
       <c r="AH9" s="4">
-        <v>44048.70492492595</v>
+        <v>215.2527280272866</v>
       </c>
       <c r="AI9" s="4">
-        <v>215.2451075129761</v>
+        <v>0.6979624794027917</v>
       </c>
       <c r="AJ9" s="4">
-        <v>0.6979624794027917</v>
+        <v>1.333396989833812</v>
       </c>
       <c r="AK9" s="4">
-        <v>1.333396989833812</v>
+        <v>0.9955885374122334</v>
       </c>
       <c r="AL9" s="4">
-        <v>0.9981982545855603</v>
+        <v>0.002318004343065792</v>
       </c>
       <c r="AM9" s="4">
-        <v>0.002324080483473825</v>
+        <v>0.9955885374122334</v>
       </c>
       <c r="AN9" s="4">
-        <v>0.9981982545855603</v>
+        <v>0.002318004343065791</v>
       </c>
       <c r="AO9" s="4">
-        <v>0.002324080483473824</v>
-      </c>
-      <c r="AP9" s="4">
-        <v>642.115</v>
+        <v>570.2877</v>
+      </c>
+      <c r="AP9" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="AQ9" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AR9" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="AR9" s="4">
+        <v>2.26011932166647E-05</v>
       </c>
       <c r="AS9" s="4">
-        <v>2.266123955941114E-05</v>
+        <v>9.717481944127452E-08</v>
       </c>
       <c r="AT9" s="4">
-        <v>9.743299132001371E-08</v>
+        <v>8</v>
       </c>
       <c r="AU9" s="4">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV9" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="AW9" s="4">
-        <v>642.1132</v>
-      </c>
-      <c r="AX9" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AY9" s="4">
-        <v>116.7139883912944</v>
+        <v>570.268</v>
+      </c>
+      <c r="AW9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AX9" s="4">
+        <v>60.16809910079359</v>
+      </c>
+      <c r="AY9" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="AZ9" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BA9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="BC9" s="4">
-        <v>4.285403036094117</v>
-      </c>
-      <c r="BD9" s="4" t="s">
-        <v>119</v>
+      <c r="BB9" s="4">
+        <v>3.497885056565243</v>
+      </c>
+      <c r="BC9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BD9" s="4">
+        <v>570210</v>
       </c>
       <c r="BE9" s="4">
-        <v>642055.2</v>
+        <v>30084.04955039679</v>
       </c>
       <c r="BF9" s="4">
-        <v>58356.99419564722</v>
-      </c>
-      <c r="BG9" s="4">
-        <v>9088.272004943556</v>
+        <v>10.5508461110905</v>
       </c>
     </row>
-    <row r="10" spans="1:59">
+    <row r="10" spans="1:58">
       <c r="A10">
         <v>10992</v>
       </c>
@@ -3591,10 +3557,10 @@
         <v>0.0001451909346112916</v>
       </c>
       <c r="Q10">
-        <v>2.46877500107601</v>
+        <v>2.12944078040521</v>
       </c>
       <c r="R10">
-        <v>0.008079781575073844</v>
+        <v>0.0001083328706218545</v>
       </c>
       <c r="S10">
         <v>1.145993042881479</v>
@@ -3612,115 +3578,112 @@
         <v>0.003</v>
       </c>
       <c r="X10">
-        <v>0.1295900854374632</v>
+        <v>0.1291711212722189</v>
       </c>
       <c r="Y10">
-        <v>0.0003235275340622288</v>
+        <v>0.0003224815709950363</v>
       </c>
       <c r="Z10">
-        <v>3.164293330984982E-05</v>
+        <v>3.154063184831989E-05</v>
       </c>
       <c r="AA10">
-        <v>7.899802017779792E-08</v>
+        <v>7.874261993272505E-08</v>
       </c>
       <c r="AB10">
         <v>0.05</v>
       </c>
       <c r="AC10">
-        <v>0.85</v>
+        <v>0.05616627403722003</v>
       </c>
       <c r="AD10">
-        <v>0.05548268026115982</v>
+        <v>0.001199923066243893</v>
       </c>
       <c r="AE10">
-        <v>0.001185318929617492</v>
+        <v>0.00256059759077345</v>
       </c>
       <c r="AF10">
-        <v>0.002529432828537529</v>
+        <v>5.470400458648045E-05</v>
       </c>
       <c r="AG10">
-        <v>5.403820793712274E-05</v>
+        <v>81.18409304821357</v>
       </c>
       <c r="AH10">
-        <v>79.93673670418434</v>
+        <v>1.746200174896844</v>
       </c>
       <c r="AI10">
-        <v>1.719370610331665</v>
+        <v>145.1899155599503</v>
       </c>
       <c r="AJ10">
-        <v>145.1899155599503</v>
+        <v>0.3791130483964922</v>
       </c>
       <c r="AK10">
-        <v>0.3791130483964922</v>
+        <v>0.001202474196200091</v>
       </c>
       <c r="AL10">
-        <v>0.001187839010041033</v>
+        <v>2.56894487010916E-05</v>
       </c>
       <c r="AM10">
-        <v>2.537678514020011E-05</v>
+        <v>0.001208645218730392</v>
       </c>
       <c r="AN10">
-        <v>0.001190813506301221</v>
+        <v>2.582128534858592E-05</v>
       </c>
       <c r="AO10">
-        <v>2.544033175877136E-05</v>
+        <v>0.1146</v>
       </c>
       <c r="AP10">
-        <v>0.1132</v>
+        <v>0.0053</v>
       </c>
       <c r="AQ10">
-        <v>0.0041</v>
+        <v>4.62478184991274</v>
       </c>
       <c r="AR10">
-        <v>3.621908127208481</v>
+        <v>1.481169710778153E-05</v>
       </c>
       <c r="AS10">
-        <v>1.485973857597886E-05</v>
+        <v>3.698575134213195E-08</v>
       </c>
       <c r="AT10">
-        <v>3.710571394897759E-08</v>
+        <v>8</v>
       </c>
       <c r="AU10">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV10">
-        <v>0.375</v>
+        <v>0.104</v>
       </c>
       <c r="AW10">
-        <v>0.1125</v>
+        <v>0.0060902994</v>
       </c>
       <c r="AX10">
-        <v>0.0024970861</v>
+        <v>0.006164045001151234</v>
       </c>
       <c r="AY10">
-        <v>0.002485978377922835</v>
-      </c>
-      <c r="AZ10">
-        <v>2.219632088888889</v>
-      </c>
-      <c r="BA10" t="s">
+        <v>5.856057115384615</v>
+      </c>
+      <c r="AZ10" t="s">
         <v>29</v>
       </c>
+      <c r="BA10">
+        <v>83.5</v>
+      </c>
       <c r="BB10">
-        <v>83.5</v>
+        <v>145.232598259485</v>
       </c>
       <c r="BC10">
-        <v>145.2360873039804</v>
+        <v>0.3792327391359274</v>
       </c>
       <c r="BD10">
-        <v>0.3792349950813442</v>
+        <v>46</v>
       </c>
       <c r="BE10">
-        <v>54.5</v>
+        <v>3.082022500575617</v>
       </c>
       <c r="BF10">
-        <v>1.242989188961417</v>
-      </c>
-      <c r="BG10">
-        <v>1104.879279076815</v>
+        <v>5.926966347260803</v>
       </c>
     </row>
-    <row r="11" spans="1:59" s="4" customFormat="1">
+    <row r="11" spans="1:58" s="4" customFormat="1">
       <c r="A11" s="4">
         <v>10815</v>
       </c>
@@ -3770,10 +3733,10 @@
         <v>0.001369559056425418</v>
       </c>
       <c r="Q11" s="4">
-        <v>10.54823824316198</v>
+        <v>10.22012575559913</v>
       </c>
       <c r="R11" s="4">
-        <v>0.09718124234229489</v>
+        <v>0.001021883800568808</v>
       </c>
       <c r="S11" s="4">
         <v>1.00070464735957</v>
@@ -3791,112 +3754,109 @@
         <v>0</v>
       </c>
       <c r="X11" s="4">
-        <v>0.9495096631476283</v>
+        <v>0.9469937115146677</v>
       </c>
       <c r="Y11" s="4">
-        <v>0.003940845703745954</v>
+        <v>0.003930403495974505</v>
       </c>
       <c r="Z11" s="4">
-        <v>0.0002318485310555446</v>
+        <v>0.0002312341932420937</v>
       </c>
       <c r="AA11" s="4">
-        <v>9.622643381018397E-07</v>
+        <v>9.597145899247003E-07</v>
       </c>
       <c r="AB11" s="4">
         <v>0</v>
       </c>
       <c r="AC11" s="4">
-        <v>0.85</v>
+        <v>222.8764989630502</v>
       </c>
       <c r="AD11" s="4">
-        <v>223.4607069138011</v>
+        <v>0.5469314400165655</v>
       </c>
       <c r="AE11" s="4">
-        <v>0.5483650666988755</v>
+        <v>10.16084894480664</v>
       </c>
       <c r="AF11" s="4">
-        <v>10.1874827476865</v>
+        <v>0.02493438191567796</v>
       </c>
       <c r="AG11" s="4">
-        <v>0.02499974037307463</v>
+        <v>43941.80982640664</v>
       </c>
       <c r="AH11" s="4">
-        <v>43940.25142754022</v>
+        <v>211.8696100379835</v>
       </c>
       <c r="AI11" s="4">
-        <v>211.8620960698193</v>
+        <v>0.7046473595699876</v>
       </c>
       <c r="AJ11" s="4">
-        <v>0.7046473595699876</v>
+        <v>1.929450337261307</v>
       </c>
       <c r="AK11" s="4">
-        <v>1.929450337261307</v>
+        <v>0.9941999920343429</v>
       </c>
       <c r="AL11" s="4">
-        <v>0.996806007216227</v>
+        <v>0.00244175772607275</v>
       </c>
       <c r="AM11" s="4">
-        <v>0.002448158106032126</v>
+        <v>0.9941999920343429</v>
       </c>
       <c r="AN11" s="4">
-        <v>0.996806007216227</v>
+        <v>0.00244175772607275</v>
       </c>
       <c r="AO11" s="4">
-        <v>0.002448158106032126</v>
-      </c>
-      <c r="AP11" s="4">
-        <v>597.8621000000001</v>
+        <v>545.198</v>
+      </c>
+      <c r="AP11" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="AQ11" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AR11" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="AR11" s="4">
+        <v>2.262537651412079E-05</v>
       </c>
       <c r="AS11" s="4">
-        <v>2.268548710650899E-05</v>
+        <v>9.39316277310498E-08</v>
       </c>
       <c r="AT11" s="4">
-        <v>9.418118317086215E-08</v>
+        <v>8</v>
       </c>
       <c r="AU11" s="4">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV11" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="AW11" s="4">
-        <v>597.8603000000001</v>
-      </c>
-      <c r="AX11" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AY11" s="4">
-        <v>95.15065789542476</v>
+        <v>545.1783</v>
+      </c>
+      <c r="AW11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AX11" s="4">
+        <v>58.40674049930108</v>
+      </c>
+      <c r="AY11" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="AZ11" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BA11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="BC11" s="4">
-        <v>3.817801622193539</v>
-      </c>
-      <c r="BD11" s="4" t="s">
-        <v>119</v>
+      <c r="BB11" s="4">
+        <v>3.289644909756741</v>
+      </c>
+      <c r="BC11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BD11" s="4">
+        <v>545120.3</v>
       </c>
       <c r="BE11" s="4">
-        <v>597802.3</v>
+        <v>29203.37024965054</v>
       </c>
       <c r="BF11" s="4">
-        <v>47575.32894771238</v>
-      </c>
-      <c r="BG11" s="4">
-        <v>7957.599617789035</v>
+        <v>10.71332818993366</v>
       </c>
     </row>
-    <row r="12" spans="1:59">
+    <row r="12" spans="1:58">
       <c r="A12">
         <v>10993</v>
       </c>
@@ -3946,10 +3906,10 @@
         <v>0.000175883451104777</v>
       </c>
       <c r="Q12">
-        <v>2.359596720214717</v>
+        <v>2.040633351441099</v>
       </c>
       <c r="R12">
-        <v>0.00844232571715587</v>
+        <v>0.0001312338074279276</v>
       </c>
       <c r="S12">
         <v>1.146960467703163</v>
@@ -3967,115 +3927,112 @@
         <v>0.003</v>
       </c>
       <c r="X12">
-        <v>0.06670335028671695</v>
+        <v>0.06643871873194153</v>
       </c>
       <c r="Y12">
-        <v>0.0002422363215640647</v>
+        <v>0.0002412752997544699</v>
       </c>
       <c r="Z12">
-        <v>1.628743169310356E-05</v>
+        <v>1.622281472328544E-05</v>
       </c>
       <c r="AA12">
-        <v>5.914856636292595E-08</v>
+        <v>5.891390682915326E-08</v>
       </c>
       <c r="AB12">
         <v>0.05</v>
       </c>
       <c r="AC12">
-        <v>0.85</v>
+        <v>0.06867324615603854</v>
       </c>
       <c r="AD12">
-        <v>0.0679031344882874</v>
+        <v>0.001554011354629662</v>
       </c>
       <c r="AE12">
-        <v>0.001536584447602451</v>
+        <v>0.003130785363138321</v>
       </c>
       <c r="AF12">
-        <v>0.003095676285406668</v>
+        <v>7.084674564779532E-05</v>
       </c>
       <c r="AG12">
-        <v>7.005226004387333E-05</v>
+        <v>192.9865696268197</v>
       </c>
       <c r="AH12">
-        <v>190.0653426357847</v>
+        <v>4.422984055694778</v>
       </c>
       <c r="AI12">
-        <v>4.356033591580113</v>
+        <v>145.9144393217995</v>
       </c>
       <c r="AJ12">
-        <v>145.9144393217995</v>
+        <v>0.4876883458809652</v>
       </c>
       <c r="AK12">
-        <v>0.4876883458809652</v>
+        <v>0.001534222382931924</v>
       </c>
       <c r="AL12">
-        <v>0.001517017392281909</v>
+        <v>3.471815830972342E-05</v>
       </c>
       <c r="AM12">
-        <v>3.432882388483839E-05</v>
+        <v>0.001543690821823429</v>
       </c>
       <c r="AN12">
-        <v>0.001522389152914374</v>
+        <v>3.493242109459623E-05</v>
       </c>
       <c r="AO12">
-        <v>3.445038229652278E-05</v>
+        <v>0.1462</v>
       </c>
       <c r="AP12">
-        <v>0.1445</v>
+        <v>0.0051</v>
       </c>
       <c r="AQ12">
-        <v>0.0056</v>
+        <v>3.488372093023257</v>
       </c>
       <c r="AR12">
-        <v>3.875432525951557</v>
+        <v>7.949891984186606E-06</v>
       </c>
       <c r="AS12">
-        <v>7.981557138425357E-06</v>
+        <v>2.887492935027594E-08</v>
       </c>
       <c r="AT12">
-        <v>2.898994086154279E-08</v>
+        <v>8</v>
       </c>
       <c r="AU12">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV12">
-        <v>0.375</v>
+        <v>0.1411</v>
       </c>
       <c r="AW12">
-        <v>0.1446</v>
+        <v>0.004549425</v>
       </c>
       <c r="AX12">
-        <v>0.0033411831</v>
+        <v>0.004505119180382099</v>
       </c>
       <c r="AY12">
-        <v>0.003300004180780491</v>
-      </c>
-      <c r="AZ12">
-        <v>2.310638381742739</v>
-      </c>
-      <c r="BA12" t="s">
+        <v>3.22425584691708</v>
+      </c>
+      <c r="AZ12" t="s">
         <v>30</v>
       </c>
+      <c r="BA12">
+        <v>100</v>
+      </c>
       <c r="BB12">
-        <v>100</v>
+        <v>145.9726402809931</v>
       </c>
       <c r="BC12">
-        <v>145.9740842567913</v>
+        <v>0.4878864806713097</v>
       </c>
       <c r="BD12">
-        <v>0.4878896438627063</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="BE12">
-        <v>86.59999999999999</v>
+        <v>2.25255959019105</v>
       </c>
       <c r="BF12">
-        <v>1.650002090390246</v>
-      </c>
-      <c r="BG12">
-        <v>1141.080283810682</v>
+        <v>3.192855549526647</v>
       </c>
     </row>
-    <row r="13" spans="1:59" s="4" customFormat="1">
+    <row r="13" spans="1:58" s="4" customFormat="1">
       <c r="A13" s="4">
         <v>10815</v>
       </c>
@@ -4125,10 +4082,10 @@
         <v>0.001565780238667443</v>
       </c>
       <c r="Q13" s="4">
-        <v>10.39473298708381</v>
+        <v>10.22078071855752</v>
       </c>
       <c r="R13" s="4">
-        <v>0.08797657437095568</v>
+        <v>0.001168292417649501</v>
       </c>
       <c r="S13" s="4">
         <v>1.00112101840651</v>
@@ -4146,109 +4103,106 @@
         <v>0</v>
       </c>
       <c r="X13" s="4">
-        <v>0.9460097571967889</v>
+        <v>0.9435030793968748</v>
       </c>
       <c r="Y13" s="4">
-        <v>0.003905245893711661</v>
+        <v>0.003894898016102048</v>
       </c>
       <c r="Z13" s="4">
-        <v>0.0002309939341145881</v>
+        <v>0.0002303818607589436</v>
       </c>
       <c r="AA13" s="4">
-        <v>9.535716791614916E-07</v>
+        <v>9.510449642512102E-07</v>
       </c>
       <c r="AB13" s="4">
         <v>0</v>
       </c>
       <c r="AC13" s="4">
-        <v>0.85</v>
+        <v>222.7411888959962</v>
       </c>
       <c r="AD13" s="4">
-        <v>223.3250373579986</v>
+        <v>0.5821115409793647</v>
       </c>
       <c r="AE13" s="4">
-        <v>0.5836373698105709</v>
+        <v>10.15468021387967</v>
       </c>
       <c r="AF13" s="4">
-        <v>10.18129762781369</v>
+        <v>0.02653822841097538</v>
       </c>
       <c r="AG13" s="4">
-        <v>0.02660779032684201</v>
+        <v>44077.60307355473</v>
       </c>
       <c r="AH13" s="4">
-        <v>44076.03890915638</v>
+        <v>215.3553534630865</v>
       </c>
       <c r="AI13" s="4">
-        <v>215.3477112331694</v>
+        <v>1.121018406509577</v>
       </c>
       <c r="AJ13" s="4">
-        <v>1.121018406509577</v>
+        <v>1.506192629674534</v>
       </c>
       <c r="AK13" s="4">
-        <v>1.506192629674534</v>
+        <v>0.9935327342892867</v>
       </c>
       <c r="AL13" s="4">
-        <v>0.9961369789812493</v>
+        <v>0.00259897960194146</v>
       </c>
       <c r="AM13" s="4">
-        <v>0.002605792038612424</v>
+        <v>0.9935327342892867</v>
       </c>
       <c r="AN13" s="4">
-        <v>0.9961369789812493</v>
+        <v>0.00259897960194146</v>
       </c>
       <c r="AO13" s="4">
-        <v>0.002605792038612424</v>
-      </c>
-      <c r="AP13" s="4">
-        <v>569.3471</v>
+        <v>526.8188</v>
+      </c>
+      <c r="AP13" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="AQ13" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AR13" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="AR13" s="4">
+        <v>2.254053453476868E-05</v>
       </c>
       <c r="AS13" s="4">
-        <v>2.260041972089083E-05</v>
+        <v>9.308579324971961E-08</v>
       </c>
       <c r="AT13" s="4">
-        <v>9.333310149547077E-08</v>
+        <v>8</v>
       </c>
       <c r="AU13" s="4">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="AV13" s="4">
-        <v>0.375</v>
+        <v>526.7992</v>
       </c>
       <c r="AW13" s="4">
-        <v>569.3452</v>
-      </c>
-      <c r="AX13" s="4" t="s">
-        <v>119</v>
+        <v>48.3631223366</v>
+      </c>
+      <c r="AX13" s="4">
+        <v>45.21647771575007</v>
       </c>
       <c r="AY13" s="4">
-        <v>67.04159439869828</v>
+        <v>9.180561082211209</v>
       </c>
       <c r="AZ13" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BA13" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="BB13" s="4">
+        <v>4.968560412105498</v>
+      </c>
       <c r="BC13" s="4">
-        <v>5.603424352859182</v>
-      </c>
-      <c r="BD13" s="4" t="s">
-        <v>119</v>
+        <v>6.710180727175612</v>
+      </c>
+      <c r="BD13" s="4">
+        <v>526741.2000000001</v>
       </c>
       <c r="BE13" s="4">
-        <v>569287.2</v>
+        <v>22608.23885787503</v>
       </c>
       <c r="BF13" s="4">
-        <v>33520.79719934914</v>
-      </c>
-      <c r="BG13" s="4">
-        <v>5887.605129427478</v>
+        <v>8.58324722508122</v>
       </c>
     </row>
   </sheetData>
@@ -4272,15 +4226,15 @@
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
     <col min="13" max="13" width="16.7109375" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" customWidth="1"/>
     <col min="18" max="18" width="20.7109375" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" customWidth="1"/>
   </cols>
@@ -4293,52 +4247,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>4</v>
@@ -4346,55 +4300,55 @@
     </row>
     <row r="2" spans="1:19" s="3" customFormat="1">
       <c r="C2" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="4" customFormat="1">
@@ -4411,22 +4365,22 @@
         <v>0.001458381816529189</v>
       </c>
       <c r="E3" s="4">
-        <v>0.9308953049971663</v>
+        <v>0.9284286765323656</v>
       </c>
       <c r="F3" s="4">
-        <v>0.004344705994292121</v>
+        <v>0.004333193662648399</v>
       </c>
       <c r="G3" s="4">
-        <v>1.002044224632932</v>
+        <v>0.9994243199508722</v>
       </c>
       <c r="H3" s="4">
-        <v>0.003417633598299903</v>
+        <v>0.003408697990423883</v>
       </c>
       <c r="I3" s="4">
-        <v>45066.6794231648</v>
+        <v>45068.26898406901</v>
       </c>
       <c r="J3" s="4">
-        <v>260.4696265987955</v>
+        <v>260.4788137042241</v>
       </c>
       <c r="K3" s="4">
         <v>0.1143667343042054</v>
@@ -4434,23 +4388,23 @@
       <c r="L3" s="4">
         <v>1.672089322806292</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>118</v>
+      <c r="M3" s="4">
+        <v>787.196</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>118</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>0.1143667343042054</v>
-      </c>
-      <c r="R3" s="4">
-        <v>1.672089322806292</v>
+        <v>116</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -4467,22 +4421,22 @@
         <v>0.0001619437037934368</v>
       </c>
       <c r="E4">
-        <v>0.1648649603714585</v>
+        <v>0.164348706667991</v>
       </c>
       <c r="F4">
-        <v>0.0003275915424590783</v>
+        <v>0.0003265657311123974</v>
       </c>
       <c r="G4">
-        <v>0.001275152828087398</v>
+        <v>0.001293671958225894</v>
       </c>
       <c r="H4">
-        <v>2.701597863848178E-05</v>
+        <v>2.740833351015257E-05</v>
       </c>
       <c r="I4">
-        <v>0.001518292136678262</v>
+        <v>69.26810743394481</v>
       </c>
       <c r="J4">
-        <v>3.230829199979801E-05</v>
+        <v>1.473981315707428</v>
       </c>
       <c r="K4">
         <v>145.9064109889343</v>
@@ -4491,22 +4445,22 @@
         <v>0.5483315951927344</v>
       </c>
       <c r="M4">
-        <v>0.1218</v>
+        <v>0.1232</v>
       </c>
       <c r="N4">
-        <v>0.0032</v>
+        <v>0.0041</v>
       </c>
       <c r="O4">
-        <v>0.1202</v>
+        <v>0.1091</v>
       </c>
       <c r="P4">
-        <v>0.0026814172</v>
+        <v>0.0076270048</v>
       </c>
       <c r="Q4">
-        <v>145.9064109889343</v>
+        <v>145.9514080700588</v>
       </c>
       <c r="R4">
-        <v>0.5483315951927344</v>
+        <v>0.5485097219309453</v>
       </c>
       <c r="S4">
         <v>30</v>
@@ -4526,22 +4480,22 @@
         <v>0.001718799455033931</v>
       </c>
       <c r="E5" s="4">
-        <v>0.9350241754877243</v>
+        <v>0.9325466065987698</v>
       </c>
       <c r="F5" s="4">
-        <v>0.003866776386707385</v>
+        <v>0.003856530443204103</v>
       </c>
       <c r="G5" s="4">
-        <v>1.001071669639563</v>
+        <v>0.9984543410506036</v>
       </c>
       <c r="H5" s="4">
-        <v>0.002858641065203783</v>
+        <v>0.002851167071869993</v>
       </c>
       <c r="I5" s="4">
-        <v>44825.30040817269</v>
+        <v>44826.88294990959</v>
       </c>
       <c r="J5" s="4">
-        <v>225.203410377069</v>
+        <v>225.2113611056301</v>
       </c>
       <c r="K5" s="4">
         <v>0.07524374222045438</v>
@@ -4549,23 +4503,23 @@
       <c r="L5" s="4">
         <v>1.847658475256469</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>118</v>
+      <c r="M5" s="4">
+        <v>699.4166</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
+      </c>
+      <c r="O5" s="4">
+        <v>699.3971</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="4">
-        <v>0.07524374222045438</v>
-      </c>
-      <c r="R5" s="4">
-        <v>1.847658475256469</v>
+        <v>0.5431789176196203</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -4582,22 +4536,22 @@
         <v>0.0001723385360822908</v>
       </c>
       <c r="E6">
-        <v>0.08206535589386277</v>
+        <v>0.08175910603621016</v>
       </c>
       <c r="F6">
-        <v>0.0002542747168099036</v>
+        <v>0.0002533258194953242</v>
       </c>
       <c r="G6">
-        <v>0.001202215160090243</v>
+        <v>0.001222639286764136</v>
       </c>
       <c r="H6">
-        <v>2.40145396881105E-05</v>
+        <v>2.442251657684677E-05</v>
       </c>
       <c r="I6">
-        <v>0.002908097732725629</v>
+        <v>131.9838503807886</v>
       </c>
       <c r="J6">
-        <v>5.878438272459443E-05</v>
+        <v>2.667925870214171</v>
       </c>
       <c r="K6">
         <v>144.4746150985909</v>
@@ -4606,22 +4560,22 @@
         <v>0.4966198109484972</v>
       </c>
       <c r="M6">
-        <v>0.1147</v>
+        <v>0.1163</v>
       </c>
       <c r="N6">
-        <v>0.0052</v>
+        <v>0.0044</v>
       </c>
       <c r="O6">
-        <v>0.1141</v>
+        <v>0.1097</v>
       </c>
       <c r="P6">
-        <v>0.0023327735</v>
+        <v>0.0042628134</v>
       </c>
       <c r="Q6">
-        <v>144.4746150985909</v>
+        <v>144.5194156912648</v>
       </c>
       <c r="R6">
-        <v>0.4966198109484972</v>
+        <v>0.4967768607109589</v>
       </c>
       <c r="S6">
         <v>47.5</v>
@@ -4641,22 +4595,22 @@
         <v>0.001771577620583448</v>
       </c>
       <c r="E7" s="4">
-        <v>0.9446978553457307</v>
+        <v>0.9421946537417234</v>
       </c>
       <c r="F7" s="4">
-        <v>0.00359360536525734</v>
+        <v>0.003584083253331734</v>
       </c>
       <c r="G7" s="4">
-        <v>1.000062521595576</v>
+        <v>0.9974478616314266</v>
       </c>
       <c r="H7" s="4">
-        <v>0.002213653272754594</v>
+        <v>0.002207865684017097</v>
       </c>
       <c r="I7" s="4">
-        <v>44328.29804948058</v>
+        <v>44329.86438603393</v>
       </c>
       <c r="J7" s="4">
-        <v>195.0099897970511</v>
+        <v>195.0168804580674</v>
       </c>
       <c r="K7" s="4">
         <v>2.514640426850789</v>
@@ -4665,22 +4619,22 @@
         <v>1.802158364614082</v>
       </c>
       <c r="M7" s="4">
-        <v>617.4591</v>
+        <v>557.1646</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O7" s="4">
-        <v>617.4573</v>
+        <v>557.1452</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q7" s="4">
-        <v>2.514640426850789</v>
-      </c>
-      <c r="R7" s="4">
-        <v>1.802158364614082</v>
+        <v>12.14344236039566</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -4697,22 +4651,22 @@
         <v>0.0001972308851365691</v>
       </c>
       <c r="E8">
-        <v>0.06829703125084907</v>
+        <v>0.06804359221735705</v>
       </c>
       <c r="F8">
-        <v>0.0002631033824980844</v>
+        <v>0.0002621270491824548</v>
       </c>
       <c r="G8">
-        <v>0.001360027298009095</v>
+        <v>0.00137769211062768</v>
       </c>
       <c r="H8">
-        <v>2.633488345141829E-05</v>
+        <v>2.667693598388037E-05</v>
       </c>
       <c r="I8">
-        <v>0.003791374615280947</v>
+        <v>169.8979652113942</v>
       </c>
       <c r="J8">
-        <v>7.485256531923752E-05</v>
+        <v>3.354271162584406</v>
       </c>
       <c r="K8">
         <v>144.5202595351331</v>
@@ -4721,22 +4675,22 @@
         <v>0.5464885728009569</v>
       </c>
       <c r="M8">
-        <v>0.1295</v>
+        <v>0.1309</v>
       </c>
       <c r="N8">
         <v>0.0026</v>
       </c>
       <c r="O8">
-        <v>0.1293</v>
+        <v>0.1254</v>
       </c>
       <c r="P8">
-        <v>0.0025250226</v>
+        <v>0.0040577034</v>
       </c>
       <c r="Q8">
-        <v>144.5202595351331</v>
+        <v>144.5714891971889</v>
       </c>
       <c r="R8">
-        <v>0.5464885728009569</v>
+        <v>0.5466848067060551</v>
       </c>
       <c r="S8">
         <v>70</v>
@@ -4756,22 +4710,22 @@
         <v>0.001644691398066958</v>
       </c>
       <c r="E9" s="4">
-        <v>0.9488419428341529</v>
+        <v>0.9463277604849375</v>
       </c>
       <c r="F9" s="4">
-        <v>0.004077997428984894</v>
+        <v>0.004067191805104615</v>
       </c>
       <c r="G9" s="4">
-        <v>0.9981982545855603</v>
+        <v>0.9955885374122334</v>
       </c>
       <c r="H9" s="4">
-        <v>0.002324080483473824</v>
+        <v>0.002318004343065791</v>
       </c>
       <c r="I9" s="4">
-        <v>44048.70492492595</v>
+        <v>44050.2644204709</v>
       </c>
       <c r="J9" s="4">
-        <v>215.2451075129761</v>
+        <v>215.2527280272866</v>
       </c>
       <c r="K9" s="4">
         <v>0.6979624794027917</v>
@@ -4780,22 +4734,22 @@
         <v>1.333396989833812</v>
       </c>
       <c r="M9" s="4">
-        <v>642.115</v>
+        <v>570.2877</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O9" s="4">
-        <v>642.1132</v>
+        <v>570.268</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q9" s="4">
-        <v>0.6979624794027917</v>
-      </c>
-      <c r="R9" s="4">
-        <v>1.333396989833812</v>
+        <v>3.497885056565243</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -4812,22 +4766,22 @@
         <v>0.0001451909346112916</v>
       </c>
       <c r="E10">
-        <v>0.1295900854374632</v>
+        <v>0.1291711212722189</v>
       </c>
       <c r="F10">
-        <v>0.0003235275340622288</v>
+        <v>0.0003224815709950363</v>
       </c>
       <c r="G10">
-        <v>0.001190813506301221</v>
+        <v>0.001208645218730392</v>
       </c>
       <c r="H10">
-        <v>2.544033175877136E-05</v>
+        <v>2.582128534858592E-05</v>
       </c>
       <c r="I10">
-        <v>0.001816972038717535</v>
+        <v>81.18409304821357</v>
       </c>
       <c r="J10">
-        <v>3.908150935315588E-05</v>
+        <v>1.746200174896844</v>
       </c>
       <c r="K10">
         <v>145.1899155599503</v>
@@ -4836,22 +4790,22 @@
         <v>0.3791130483964922</v>
       </c>
       <c r="M10">
-        <v>0.1132</v>
+        <v>0.1146</v>
       </c>
       <c r="N10">
-        <v>0.0041</v>
+        <v>0.0053</v>
       </c>
       <c r="O10">
-        <v>0.1125</v>
+        <v>0.104</v>
       </c>
       <c r="P10">
-        <v>0.0024970861</v>
+        <v>0.0060902994</v>
       </c>
       <c r="Q10">
-        <v>145.1899155599503</v>
+        <v>145.232598259485</v>
       </c>
       <c r="R10">
-        <v>0.3791130483964922</v>
+        <v>0.3792327391359274</v>
       </c>
       <c r="S10">
         <v>83.5</v>
@@ -4871,22 +4825,22 @@
         <v>0.001369559056425418</v>
       </c>
       <c r="E11" s="4">
-        <v>0.9495096631476283</v>
+        <v>0.9469937115146677</v>
       </c>
       <c r="F11" s="4">
-        <v>0.003940845703745954</v>
+        <v>0.003930403495974505</v>
       </c>
       <c r="G11" s="4">
-        <v>0.996806007216227</v>
+        <v>0.9941999920343429</v>
       </c>
       <c r="H11" s="4">
-        <v>0.002448158106032126</v>
+        <v>0.00244175772607275</v>
       </c>
       <c r="I11" s="4">
-        <v>43940.25142754022</v>
+        <v>43941.80982640664</v>
       </c>
       <c r="J11" s="4">
-        <v>211.8620960698193</v>
+        <v>211.8696100379835</v>
       </c>
       <c r="K11" s="4">
         <v>0.7046473595699876</v>
@@ -4895,22 +4849,22 @@
         <v>1.929450337261307</v>
       </c>
       <c r="M11" s="4">
-        <v>597.8621000000001</v>
+        <v>545.198</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O11" s="4">
-        <v>597.8603000000001</v>
+        <v>545.1783</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q11" s="4">
-        <v>0.7046473595699876</v>
-      </c>
-      <c r="R11" s="4">
-        <v>1.929450337261307</v>
+        <v>3.289644909756741</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -4927,22 +4881,22 @@
         <v>0.000175883451104777</v>
       </c>
       <c r="E12">
-        <v>0.06670335028671695</v>
+        <v>0.06643871873194153</v>
       </c>
       <c r="F12">
-        <v>0.0002422363215640647</v>
+        <v>0.0002412752997544699</v>
       </c>
       <c r="G12">
-        <v>0.001522389152914374</v>
+        <v>0.001543690821823429</v>
       </c>
       <c r="H12">
-        <v>3.445038229652278E-05</v>
+        <v>3.493242109459623E-05</v>
       </c>
       <c r="I12">
-        <v>0.004318867380315865</v>
+        <v>192.9865696268197</v>
       </c>
       <c r="J12">
-        <v>9.898244006686914E-05</v>
+        <v>4.422984055694778</v>
       </c>
       <c r="K12">
         <v>145.9144393217995</v>
@@ -4951,22 +4905,22 @@
         <v>0.4876883458809652</v>
       </c>
       <c r="M12">
-        <v>0.1445</v>
+        <v>0.1462</v>
       </c>
       <c r="N12">
-        <v>0.0056</v>
+        <v>0.0051</v>
       </c>
       <c r="O12">
-        <v>0.1446</v>
+        <v>0.1411</v>
       </c>
       <c r="P12">
-        <v>0.0033411831</v>
+        <v>0.004549425</v>
       </c>
       <c r="Q12">
-        <v>145.9144393217995</v>
+        <v>145.9726402809931</v>
       </c>
       <c r="R12">
-        <v>0.4876883458809652</v>
+        <v>0.4878864806713097</v>
       </c>
       <c r="S12">
         <v>100</v>
@@ -4986,22 +4940,22 @@
         <v>0.001565780238667443</v>
       </c>
       <c r="E13" s="4">
-        <v>0.9460097571967889</v>
+        <v>0.9435030793968748</v>
       </c>
       <c r="F13" s="4">
-        <v>0.003905245893711661</v>
+        <v>0.003894898016102048</v>
       </c>
       <c r="G13" s="4">
-        <v>0.9961369789812493</v>
+        <v>0.9935327342892867</v>
       </c>
       <c r="H13" s="4">
-        <v>0.002605792038612424</v>
+        <v>0.00259897960194146</v>
       </c>
       <c r="I13" s="4">
-        <v>44076.03890915638</v>
+        <v>44077.60307355473</v>
       </c>
       <c r="J13" s="4">
-        <v>215.3477112331694</v>
+        <v>215.3553534630865</v>
       </c>
       <c r="K13" s="4">
         <v>1.121018406509577</v>
@@ -5010,22 +4964,22 @@
         <v>1.506192629674534</v>
       </c>
       <c r="M13" s="4">
-        <v>569.3471</v>
+        <v>526.8188</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O13" s="4">
-        <v>569.3452</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>119</v>
+        <v>526.7992</v>
+      </c>
+      <c r="P13" s="4">
+        <v>48.3631223366</v>
       </c>
       <c r="Q13" s="4">
-        <v>1.121018406509577</v>
+        <v>4.968560412105498</v>
       </c>
       <c r="R13" s="4">
-        <v>1.506192629674534</v>
+        <v>6.710180727175612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a few issues with ratios dataframe
</commit_message>
<xml_diff>
--- a/data/CPR_100221_20210210-114741/Results.xlsx
+++ b/data/CPR_100221_20210210-114741/Results.xlsx
@@ -1941,7 +1941,7 @@
     <col min="52" max="52" width="12.7109375" customWidth="1"/>
     <col min="53" max="53" width="6.7109375" customWidth="1"/>
     <col min="54" max="54" width="20.7109375" customWidth="1"/>
-    <col min="55" max="55" width="19.7109375" customWidth="1"/>
+    <col min="55" max="55" width="20.7109375" customWidth="1"/>
     <col min="56" max="56" width="19.7109375" customWidth="1"/>
     <col min="57" max="57" width="19.7109375" customWidth="1"/>
     <col min="58" max="58" width="19.7109375" customWidth="1"/>
@@ -2606,13 +2606,13 @@
         <v>0.1218</v>
       </c>
       <c r="AW4">
-        <v>0.0026896708</v>
+        <v>0.0027272113</v>
       </c>
       <c r="AX4">
         <v>0.002695172695222103</v>
       </c>
       <c r="AY4">
-        <v>2.208268308702792</v>
+        <v>2.23908973727422</v>
       </c>
       <c r="AZ4" t="s">
         <v>26</v>
@@ -2624,7 +2624,7 @@
         <v>145.9565715687178</v>
       </c>
       <c r="BC4">
-        <v>0.5485212227191195</v>
+        <v>0.5485212541680431</v>
       </c>
       <c r="BD4">
         <v>63.80000000000001</v>
@@ -2934,10 +2934,10 @@
         <v>0.1166</v>
       </c>
       <c r="AP6">
-        <v>0.0042</v>
+        <v>0.0041</v>
       </c>
       <c r="AQ6">
-        <v>3.602058319039451</v>
+        <v>3.516295025728988</v>
       </c>
       <c r="AR6">
         <v>9.243171727785967E-06</v>
@@ -2955,13 +2955,13 @@
         <v>0.1159</v>
       </c>
       <c r="AW6">
-        <v>0.0023389926</v>
+        <v>0.0023770292</v>
       </c>
       <c r="AX6">
         <v>0.002353196968169543</v>
       </c>
       <c r="AY6">
-        <v>2.018112683347713</v>
+        <v>2.050931147540984</v>
       </c>
       <c r="AZ6" t="s">
         <v>27</v>
@@ -2973,7 +2973,7 @@
         <v>144.5218771154652</v>
       </c>
       <c r="BC6">
-        <v>0.4967831862381769</v>
+        <v>0.4967832162699013</v>
       </c>
       <c r="BD6">
         <v>57.90000000000001</v>
@@ -3283,10 +3283,10 @@
         <v>0.1313</v>
       </c>
       <c r="AP8">
-        <v>0.0029</v>
+        <v>0.0028</v>
       </c>
       <c r="AQ8">
-        <v>2.208682406702208</v>
+        <v>2.132520944402132</v>
       </c>
       <c r="AR8">
         <v>8.079480474611969E-06</v>
@@ -3304,13 +3304,13 @@
         <v>0.1308</v>
       </c>
       <c r="AW8">
-        <v>0.0025624011</v>
+        <v>0.0025708419</v>
       </c>
       <c r="AX8">
         <v>0.002561699555639462</v>
       </c>
       <c r="AY8">
-        <v>1.959022247706422</v>
+        <v>1.965475458715596</v>
       </c>
       <c r="AZ8" t="s">
         <v>28</v>
@@ -3322,7 +3322,7 @@
         <v>144.5736154875932</v>
       </c>
       <c r="BC8">
-        <v>0.5466913324908758</v>
+        <v>0.5466913390873795</v>
       </c>
       <c r="BD8">
         <v>72.80000000000001</v>
@@ -3632,10 +3632,10 @@
         <v>0.1151</v>
       </c>
       <c r="AP10">
-        <v>0.0055</v>
+        <v>0.0054</v>
       </c>
       <c r="AQ10">
-        <v>4.778453518679409</v>
+        <v>4.691572545612511</v>
       </c>
       <c r="AR10">
         <v>1.480945340168126E-05</v>
@@ -3653,13 +3653,13 @@
         <v>0.1141</v>
       </c>
       <c r="AW10">
-        <v>0.0025474073</v>
+        <v>0.0025160596</v>
       </c>
       <c r="AX10">
         <v>0.002517656413905989</v>
       </c>
       <c r="AY10">
-        <v>2.232609377738826</v>
+        <v>2.205135495179667</v>
       </c>
       <c r="AZ10" t="s">
         <v>29</v>
@@ -3671,7 +3671,7 @@
         <v>145.236673811475</v>
       </c>
       <c r="BC10">
-        <v>0.3792365786174705</v>
+        <v>0.379236543461545</v>
       </c>
       <c r="BD10">
         <v>56.09999999999999</v>
@@ -4002,13 +4002,13 @@
         <v>0.1464</v>
       </c>
       <c r="AW12">
-        <v>0.0033849942</v>
+        <v>0.0033822877</v>
       </c>
       <c r="AX12">
         <v>0.003341125105867086</v>
       </c>
       <c r="AY12">
-        <v>2.312154508196722</v>
+        <v>2.310305806010929</v>
       </c>
       <c r="AZ12" t="s">
         <v>30</v>
@@ -4020,7 +4020,7 @@
         <v>145.9747362666762</v>
       </c>
       <c r="BC12">
-        <v>0.487891868488217</v>
+        <v>0.487891865302871</v>
       </c>
       <c r="BD12">
         <v>88.40000000000001</v>
@@ -4235,7 +4235,7 @@
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" customWidth="1"/>
     <col min="17" max="17" width="20.7109375" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4454,13 +4454,13 @@
         <v>0.1218</v>
       </c>
       <c r="P4">
-        <v>0.0026896708</v>
+        <v>0.0027272113</v>
       </c>
       <c r="Q4">
         <v>145.9565715687178</v>
       </c>
       <c r="R4">
-        <v>0.5485212227191195</v>
+        <v>0.5485212541680431</v>
       </c>
       <c r="S4">
         <v>30</v>
@@ -4563,19 +4563,19 @@
         <v>0.1166</v>
       </c>
       <c r="N6">
-        <v>0.0042</v>
+        <v>0.0041</v>
       </c>
       <c r="O6">
         <v>0.1159</v>
       </c>
       <c r="P6">
-        <v>0.0023389926</v>
+        <v>0.0023770292</v>
       </c>
       <c r="Q6">
         <v>144.5218771154652</v>
       </c>
       <c r="R6">
-        <v>0.4967831862381769</v>
+        <v>0.4967832162699013</v>
       </c>
       <c r="S6">
         <v>47.5</v>
@@ -4678,19 +4678,19 @@
         <v>0.1313</v>
       </c>
       <c r="N8">
-        <v>0.0029</v>
+        <v>0.0028</v>
       </c>
       <c r="O8">
         <v>0.1308</v>
       </c>
       <c r="P8">
-        <v>0.0025624011</v>
+        <v>0.0025708419</v>
       </c>
       <c r="Q8">
         <v>144.5736154875932</v>
       </c>
       <c r="R8">
-        <v>0.5466913324908758</v>
+        <v>0.5466913390873795</v>
       </c>
       <c r="S8">
         <v>70</v>
@@ -4793,19 +4793,19 @@
         <v>0.1151</v>
       </c>
       <c r="N10">
-        <v>0.0055</v>
+        <v>0.0054</v>
       </c>
       <c r="O10">
         <v>0.1141</v>
       </c>
       <c r="P10">
-        <v>0.0025474073</v>
+        <v>0.0025160596</v>
       </c>
       <c r="Q10">
         <v>145.236673811475</v>
       </c>
       <c r="R10">
-        <v>0.3792365786174705</v>
+        <v>0.379236543461545</v>
       </c>
       <c r="S10">
         <v>83.5</v>
@@ -4914,13 +4914,13 @@
         <v>0.1464</v>
       </c>
       <c r="P12">
-        <v>0.0033849942</v>
+        <v>0.0033822877</v>
       </c>
       <c r="Q12">
         <v>145.9747362666762</v>
       </c>
       <c r="R12">
-        <v>0.487891868488217</v>
+        <v>0.487891865302871</v>
       </c>
       <c r="S12">
         <v>100</v>

</xml_diff>

<commit_message>
output of tailing.xlsx output of intensities.xlsx using numba to speed up age calculation added specific constants to constants sheet in Results.xlsx added support for string labnrs
</commit_message>
<xml_diff>
--- a/data/CPR_100221_20210210-114741/Results.xlsx
+++ b/data/CPR_100221_20210210-114741/Results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="181">
   <si>
     <t>Lab. #</t>
   </si>
@@ -489,13 +489,19 @@
     </r>
   </si>
   <si>
-    <t>R34_33</t>
-  </si>
-  <si>
-    <t>R35_33</t>
-  </si>
-  <si>
-    <t>R30_29</t>
+    <t>Blank</t>
+  </si>
+  <si>
+    <t>Yield_U</t>
+  </si>
+  <si>
+    <t>Yield_Th</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <t>Tail shift</t>
   </si>
   <si>
     <t>mf48</t>
@@ -540,6 +546,18 @@
     <t>mf02</t>
   </si>
   <si>
+    <t>l230</t>
+  </si>
+  <si>
+    <t>l232</t>
+  </si>
+  <si>
+    <t>l234</t>
+  </si>
+  <si>
+    <t>l238</t>
+  </si>
+  <si>
     <t>NA</t>
   </si>
   <si>
@@ -549,28 +567,37 @@
     <t>cps</t>
   </si>
   <si>
-    <t>slope229Correction</t>
-  </si>
-  <si>
-    <t>lambda232</t>
-  </si>
-  <si>
-    <t>lambda234</t>
-  </si>
-  <si>
-    <t>lambda238</t>
-  </si>
-  <si>
-    <t>lambda230</t>
-  </si>
-  <si>
-    <t>trisp236</t>
-  </si>
-  <si>
-    <t>trisp233</t>
-  </si>
-  <si>
-    <t>trisp229</t>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>R3433</t>
+  </si>
+  <si>
+    <t>R3533</t>
+  </si>
+  <si>
+    <t>R3029</t>
+  </si>
+  <si>
+    <t>th229SubU238</t>
+  </si>
+  <si>
+    <t>th230SubU238</t>
+  </si>
+  <si>
+    <t>tri229</t>
+  </si>
+  <si>
+    <t>tri233</t>
+  </si>
+  <si>
+    <t>tri236</t>
+  </si>
+  <si>
+    <t>blank232</t>
+  </si>
+  <si>
+    <t>blank232S</t>
   </si>
   <si>
     <t>blank234</t>
@@ -585,22 +612,31 @@
     <t>blank238S</t>
   </si>
   <si>
-    <t>blank232</t>
-  </si>
-  <si>
-    <t>blank232S</t>
-  </si>
-  <si>
-    <t>chBlank230</t>
-  </si>
-  <si>
-    <t>chBlank230S</t>
+    <t>ch_blank230</t>
+  </si>
+  <si>
+    <t>ch_blank230S</t>
   </si>
   <si>
     <t>a230232_init</t>
   </si>
   <si>
     <t>a230232_init_err</t>
+  </si>
+  <si>
+    <t>standardBezeich</t>
+  </si>
+  <si>
+    <t>standardEinwaage</t>
+  </si>
+  <si>
+    <t>standardTriSp13</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>stalag</t>
   </si>
   <si>
     <t>Mean method</t>
@@ -3281,10 +3317,10 @@
         <v>643.7317</v>
       </c>
       <c r="AP7" s="3">
-        <v>273.8155</v>
+        <v>270.1318</v>
       </c>
       <c r="AQ7" s="3">
-        <v>42.53565577087473</v>
+        <v>41.96341426094132</v>
       </c>
       <c r="AR7" s="3">
         <v>2.249717611187651E-05</v>
@@ -3302,13 +3338,13 @@
         <v>643.7299</v>
       </c>
       <c r="AW7" s="3">
-        <v>355.6723</v>
+        <v>344.5467</v>
       </c>
       <c r="AX7" s="3">
         <v>134.125389457695</v>
       </c>
       <c r="AY7" s="3">
-        <v>55.25179116272213</v>
+        <v>53.52348865572346</v>
       </c>
       <c r="AZ7" s="3" t="s">
         <v>25</v>
@@ -3317,7 +3353,7 @@
         <v>6.216836768979327</v>
       </c>
       <c r="BC7" s="3">
-        <v>12.70651791065451</v>
+        <v>12.61180836448982</v>
       </c>
       <c r="BD7" s="3">
         <v>643671.9</v>
@@ -3329,10 +3365,10 @@
         <v>20.83566251275496</v>
       </c>
       <c r="BG7" s="3">
-        <v>78.06</v>
+        <v>78.96000000000001</v>
       </c>
       <c r="BH7" s="3">
-        <v>77.40000000000001</v>
+        <v>78.34</v>
       </c>
     </row>
     <row r="8" spans="1:60" s="4" customFormat="1">
@@ -3642,10 +3678,10 @@
         <v>677.0234</v>
       </c>
       <c r="AP9" s="3">
-        <v>302.3145</v>
+        <v>298.3195</v>
       </c>
       <c r="AQ9" s="3">
-        <v>44.6534787423891</v>
+        <v>44.06339574082669</v>
       </c>
       <c r="AR9" s="3">
         <v>2.25977695398533E-05</v>
@@ -3663,13 +3699,13 @@
         <v>677.0214999999999</v>
       </c>
       <c r="AW9" s="3">
-        <v>400.355</v>
+        <v>400.3249</v>
       </c>
       <c r="AX9" s="3">
         <v>163.3523248281124</v>
       </c>
       <c r="AY9" s="3">
-        <v>59.13475421386175</v>
+        <v>59.13030826938288</v>
       </c>
       <c r="AZ9" s="3" t="s">
         <v>25</v>
@@ -3678,7 +3714,7 @@
         <v>-5.427845977547987</v>
       </c>
       <c r="BC9" s="3">
-        <v>10.88774112509683</v>
+        <v>10.88748143802084</v>
       </c>
       <c r="BD9" s="3">
         <v>676963.5</v>
@@ -3690,10 +3726,10 @@
         <v>24.12808527175465</v>
       </c>
       <c r="BG9" s="3">
-        <v>72.92</v>
+        <v>73.86</v>
       </c>
       <c r="BH9" s="3">
-        <v>73.94</v>
+        <v>73.72</v>
       </c>
     </row>
     <row r="10" spans="1:60" s="4" customFormat="1">
@@ -4003,10 +4039,10 @@
         <v>654.7945999999999</v>
       </c>
       <c r="AP11" s="3">
-        <v>287.1927</v>
+        <v>288.6347</v>
       </c>
       <c r="AQ11" s="3">
-        <v>43.85996769063154</v>
+        <v>44.08018942123226</v>
       </c>
       <c r="AR11" s="3">
         <v>2.262194917397206E-05</v>
@@ -4024,13 +4060,13 @@
         <v>654.7927</v>
       </c>
       <c r="AW11" s="3">
-        <v>388.3095</v>
+        <v>388.7997</v>
       </c>
       <c r="AX11" s="3">
         <v>162.5699946029966</v>
       </c>
       <c r="AY11" s="3">
-        <v>59.3026617431746</v>
+        <v>59.37752513123618</v>
       </c>
       <c r="AZ11" s="3" t="s">
         <v>25</v>
@@ -4039,7 +4075,7 @@
         <v>-9.569514961948167</v>
       </c>
       <c r="BC11" s="3">
-        <v>15.57176953748089</v>
+        <v>15.58068770008644</v>
       </c>
       <c r="BD11" s="3">
         <v>654734.7</v>
@@ -4051,10 +4087,10 @@
         <v>24.82770418836322</v>
       </c>
       <c r="BG11" s="3">
-        <v>74.72</v>
+        <v>74.16</v>
       </c>
       <c r="BH11" s="3">
-        <v>73.62</v>
+        <v>73.7</v>
       </c>
     </row>
     <row r="12" spans="1:60" s="4" customFormat="1">
@@ -4364,10 +4400,10 @@
         <v>599.4473</v>
       </c>
       <c r="AP13" s="3">
-        <v>206.4301</v>
+        <v>212.0804</v>
       </c>
       <c r="AQ13" s="3">
-        <v>34.43673864241277</v>
+        <v>35.37932358691081</v>
       </c>
       <c r="AR13" s="3">
         <v>2.253712004666341E-05</v>
@@ -4385,13 +4421,13 @@
         <v>599.4455</v>
       </c>
       <c r="AW13" s="3">
-        <v>228.1306</v>
+        <v>230.8497</v>
       </c>
       <c r="AX13" s="3">
         <v>86.29947674072298</v>
       </c>
       <c r="AY13" s="3">
-        <v>38.05693761985034</v>
+        <v>38.51054015752892</v>
       </c>
       <c r="AZ13" s="3" t="s">
         <v>25</v>
@@ -4400,7 +4436,7 @@
         <v>-2.067504518416635</v>
       </c>
       <c r="BC13" s="3">
-        <v>8.271962021784168</v>
+        <v>8.274529688906103</v>
       </c>
       <c r="BD13" s="3">
         <v>599387.5</v>
@@ -4412,10 +4448,10 @@
         <v>14.3965509359438</v>
       </c>
       <c r="BG13" s="3">
-        <v>88.98</v>
+        <v>88.28</v>
       </c>
       <c r="BH13" s="3">
-        <v>89.18000000000001</v>
+        <v>88.86</v>
       </c>
     </row>
   </sheetData>
@@ -4835,19 +4871,19 @@
         <v>643.7317</v>
       </c>
       <c r="N7" s="3">
-        <v>273.8155</v>
+        <v>270.1318</v>
       </c>
       <c r="O7" s="3">
         <v>643.7299</v>
       </c>
       <c r="P7" s="3">
-        <v>355.6723</v>
+        <v>344.5467</v>
       </c>
       <c r="Q7" s="3">
         <v>6.216836768979327</v>
       </c>
       <c r="R7" s="3">
-        <v>12.70651791065451</v>
+        <v>12.61180836448982</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="4" customFormat="1">
@@ -4950,19 +4986,19 @@
         <v>677.0234</v>
       </c>
       <c r="N9" s="3">
-        <v>302.3145</v>
+        <v>298.3195</v>
       </c>
       <c r="O9" s="3">
         <v>677.0214999999999</v>
       </c>
       <c r="P9" s="3">
-        <v>400.355</v>
+        <v>400.3249</v>
       </c>
       <c r="Q9" s="3">
         <v>-5.427845977547987</v>
       </c>
       <c r="R9" s="3">
-        <v>10.88774112509683</v>
+        <v>10.88748143802084</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="4" customFormat="1">
@@ -5065,19 +5101,19 @@
         <v>654.7945999999999</v>
       </c>
       <c r="N11" s="3">
-        <v>287.1927</v>
+        <v>288.6347</v>
       </c>
       <c r="O11" s="3">
         <v>654.7927</v>
       </c>
       <c r="P11" s="3">
-        <v>388.3095</v>
+        <v>388.7997</v>
       </c>
       <c r="Q11" s="3">
         <v>-9.569514961948167</v>
       </c>
       <c r="R11" s="3">
-        <v>15.57176953748089</v>
+        <v>15.58068770008644</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="4" customFormat="1">
@@ -5180,19 +5216,19 @@
         <v>599.4473</v>
       </c>
       <c r="N13" s="3">
-        <v>206.4301</v>
+        <v>212.0804</v>
       </c>
       <c r="O13" s="3">
         <v>599.4455</v>
       </c>
       <c r="P13" s="3">
-        <v>228.1306</v>
+        <v>230.8497</v>
       </c>
       <c r="Q13" s="3">
         <v>-2.067504518416635</v>
       </c>
       <c r="R13" s="3">
-        <v>8.271962021784168</v>
+        <v>8.274529688906103</v>
       </c>
     </row>
   </sheetData>
@@ -5202,13 +5238,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5216,8 +5252,8 @@
       <c r="A1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="6">
-        <v>0.002324</v>
+      <c r="B1" s="6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5225,7 +5261,7 @@
         <v>128</v>
       </c>
       <c r="B2" s="6">
-        <v>0.005066</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5233,7 +5269,7 @@
         <v>129</v>
       </c>
       <c r="B3" s="6">
-        <v>5E-05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5241,15 +5277,15 @@
         <v>130</v>
       </c>
       <c r="B4" s="6">
-        <v>1.336402435064349</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="6">
-        <v>1.008202776684838</v>
+      <c r="B5" s="6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5257,7 +5293,7 @@
         <v>132</v>
       </c>
       <c r="B6" s="6">
-        <v>0.334493224630051</v>
+        <v>1.336402435064349</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5265,7 +5301,7 @@
         <v>133</v>
       </c>
       <c r="B7" s="6">
-        <v>0.665506775369946</v>
+        <v>1.008202776684838</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5273,7 +5309,7 @@
         <v>134</v>
       </c>
       <c r="B8" s="6">
-        <v>1.025840620457897</v>
+        <v>0.334493224630051</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5281,7 +5317,7 @@
         <v>135</v>
       </c>
       <c r="B9" s="6">
-        <v>1.673784240557133</v>
+        <v>0.665506775369946</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5289,7 +5325,7 @@
         <v>136</v>
       </c>
       <c r="B10" s="6">
-        <v>0.673784240557127</v>
+        <v>1.025840620457897</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5297,7 +5333,7 @@
         <v>137</v>
       </c>
       <c r="B11" s="6">
-        <v>-0.337307116990441</v>
+        <v>1.673784240557133</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5305,7 +5341,7 @@
         <v>138</v>
       </c>
       <c r="B12" s="6">
-        <v>0.336402435064353</v>
+        <v>0.673784240557127</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5313,7 +5349,7 @@
         <v>139</v>
       </c>
       <c r="B13" s="6">
-        <v>-0.34318587041139</v>
+        <v>-0.337307116990441</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5321,7 +5357,7 @@
         <v>140</v>
       </c>
       <c r="B14" s="6">
-        <v>-1.025840620457897</v>
+        <v>0.336402435064353</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -5329,7 +5365,7 @@
         <v>141</v>
       </c>
       <c r="B15" s="6">
-        <v>0.337307116990439</v>
+        <v>-0.34318587041139</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -5337,7 +5373,7 @@
         <v>142</v>
       </c>
       <c r="B16" s="6">
-        <v>1</v>
+        <v>-1.025840620457897</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -5345,7 +5381,7 @@
         <v>143</v>
       </c>
       <c r="B17" s="6">
-        <v>0.682654750046506</v>
+        <v>0.337307116990439</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -5353,7 +5389,7 @@
         <v>144</v>
       </c>
       <c r="B18" s="6">
-        <v>6.02214129E+23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -5361,7 +5397,7 @@
         <v>145</v>
       </c>
       <c r="B19" s="6">
-        <v>137.881</v>
+        <v>0.682654750046506</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -5369,7 +5405,7 @@
         <v>146</v>
       </c>
       <c r="B20" s="6">
-        <v>62500000</v>
+        <v>9.1705E-06</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -5377,7 +5413,7 @@
         <v>147</v>
       </c>
       <c r="B21" s="6">
-        <v>3.4053</v>
+        <v>4.94752E-11</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -5385,7 +5421,7 @@
         <v>148</v>
       </c>
       <c r="B22" s="6">
-        <v>4.94752E-11</v>
+        <v>2.82206E-06</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -5393,7 +5429,7 @@
         <v>149</v>
       </c>
       <c r="B23" s="6">
-        <v>2.82206E-06</v>
+        <v>1.55125E-10</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -5401,7 +5437,7 @@
         <v>150</v>
       </c>
       <c r="B24" s="6">
-        <v>1.55125E-10</v>
+        <v>6.02214129E+23</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -5409,7 +5445,7 @@
         <v>151</v>
       </c>
       <c r="B25" s="6">
-        <v>9.1705E-06</v>
+        <v>137.881</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -5417,7 +5453,7 @@
         <v>152</v>
       </c>
       <c r="B26" s="6">
-        <v>3.86778</v>
+        <v>62500000</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -5425,7 +5461,7 @@
         <v>153</v>
       </c>
       <c r="B27" s="6">
-        <v>0.038556</v>
+        <v>3.4053</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5433,7 +5469,7 @@
         <v>154</v>
       </c>
       <c r="B28" s="6">
-        <v>0.018067</v>
+        <v>0.002324</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -5441,7 +5477,7 @@
         <v>155</v>
       </c>
       <c r="B29" s="6">
-        <v>0.3</v>
+        <v>0.005066</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -5449,7 +5485,7 @@
         <v>156</v>
       </c>
       <c r="B30" s="6">
-        <v>0</v>
+        <v>5E-05</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -5457,7 +5493,7 @@
         <v>157</v>
       </c>
       <c r="B31" s="6">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -5473,7 +5509,7 @@
         <v>159</v>
       </c>
       <c r="B33" s="6">
-        <v>0.003</v>
+        <v>0.018067</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -5481,7 +5517,7 @@
         <v>160</v>
       </c>
       <c r="B34" s="6">
-        <v>0</v>
+        <v>0.038556</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -5489,7 +5525,7 @@
         <v>161</v>
       </c>
       <c r="B35" s="6">
-        <v>0.05</v>
+        <v>3.86778</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -5497,7 +5533,7 @@
         <v>162</v>
       </c>
       <c r="B36" s="6">
-        <v>0</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -5505,7 +5541,7 @@
         <v>163</v>
       </c>
       <c r="B37" s="6">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -5513,7 +5549,95 @@
         <v>164</v>
       </c>
       <c r="B38" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="6">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="6">
         <v>0.375</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="6">
+        <v>1.10995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B48" s="6">
+        <v>10.34908</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -5535,18 +5659,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>